<commit_message>
Remove unused names from name manager
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_Hydrogen.xlsx
+++ b/SubRES_TMPL/SubRES_Hydrogen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D1D3C1-6A8C-4F27-977E-6D2F9290367A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56188274-7A1E-481C-AEA8-6209693E48D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,107 +19,14 @@
     <sheet name="SUP_H2Delivery" sheetId="4" r:id="rId4"/>
     <sheet name="SUP_H2Storage" sheetId="11" r:id="rId5"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId6"/>
-    <externalReference r:id="rId7"/>
-    <externalReference r:id="rId8"/>
-    <externalReference r:id="rId9"/>
-    <externalReference r:id="rId10"/>
-    <externalReference r:id="rId11"/>
-    <externalReference r:id="rId12"/>
-  </externalReferences>
   <definedNames>
     <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="All_TP">#REF!,#REF!,#REF!</definedName>
-    <definedName name="All_US">#REF!,#REF!,#REF!</definedName>
-    <definedName name="Annual_Fuel_Consumption">#REF!</definedName>
-    <definedName name="Beta">#REF!</definedName>
-    <definedName name="body1ea">#REF!</definedName>
-    <definedName name="body1eb">#REF!</definedName>
-    <definedName name="body1fa">#REF!</definedName>
-    <definedName name="body1fb">#REF!</definedName>
-    <definedName name="body1ga">#REF!</definedName>
-    <definedName name="body1gb">#REF!</definedName>
-    <definedName name="body2ea">#REF!</definedName>
-    <definedName name="body2eb">#REF!</definedName>
-    <definedName name="body2f">#REF!</definedName>
-    <definedName name="body2fa">#REF!</definedName>
-    <definedName name="body2fb">#REF!</definedName>
-    <definedName name="body2ga">#REF!</definedName>
-    <definedName name="body2gb">#REF!</definedName>
-    <definedName name="body3ea">#REF!</definedName>
-    <definedName name="body3eb">#REF!</definedName>
-    <definedName name="body3fa">#REF!</definedName>
-    <definedName name="body3fb">#REF!</definedName>
-    <definedName name="body3ga">#REF!</definedName>
-    <definedName name="body3gb">#REF!</definedName>
-    <definedName name="body4ea">#REF!</definedName>
-    <definedName name="body4eb">#REF!</definedName>
-    <definedName name="body4f">#REF!</definedName>
-    <definedName name="body4fa">#REF!</definedName>
-    <definedName name="body4fb">#REF!</definedName>
-    <definedName name="body4ga">#REF!</definedName>
-    <definedName name="body4gb">#REF!</definedName>
-    <definedName name="Cadmium_Content_ppm_wt">#REF!</definedName>
-    <definedName name="ChosenYear">[1]Cover!$G$117</definedName>
-    <definedName name="Chromium_Content_ppm_wt">#REF!</definedName>
-    <definedName name="Copper_Content_ppm_wt">#REF!</definedName>
-    <definedName name="countrye">#REF!</definedName>
-    <definedName name="countryf">#REF!</definedName>
-    <definedName name="countryg">#REF!</definedName>
-    <definedName name="CRF_CountryName">[2]Sheet1!$C$4</definedName>
-    <definedName name="data_range">'[3]CSO data'!#REF!</definedName>
     <definedName name="elec" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="EnergyService">[4]Tertiary!#REF!</definedName>
-    <definedName name="Eng">[1]Cover!$G$111</definedName>
-    <definedName name="Etiket">#REF!</definedName>
-    <definedName name="Evap_Control_perc">#REF!</definedName>
-    <definedName name="Evap_H_Share_perc">#REF!</definedName>
-    <definedName name="Evap_R_Share_perc">#REF!</definedName>
-    <definedName name="Evap_U_Share_perc">#REF!</definedName>
-    <definedName name="FID_1">[5]AGR_Fuels!$A$2</definedName>
-    <definedName name="Fuel_Injection_perc">#REF!</definedName>
-    <definedName name="Fuel_Specifications">#REF!</definedName>
-    <definedName name="H_C_Ratio">#REF!</definedName>
-    <definedName name="H_Share_perc">#REF!</definedName>
-    <definedName name="H_Speed_km_per_h">#REF!</definedName>
-    <definedName name="Improved_Fuel_Specs">#REF!</definedName>
-    <definedName name="Lead_Content_g_per_l">#REF!</definedName>
-    <definedName name="Max_Temperature_oC">#REF!</definedName>
-    <definedName name="Mean_Fleet_Mileage_km">#REF!</definedName>
-    <definedName name="Mileage_km">#REF!</definedName>
-    <definedName name="Mileage_km_per_year">#REF!</definedName>
-    <definedName name="Min_Temperature_oC">#REF!</definedName>
-    <definedName name="Nikel_Content_ppm_wt">#REF!</definedName>
-    <definedName name="O_C_Ratio">#REF!</definedName>
-    <definedName name="Population">#REF!</definedName>
-    <definedName name="qr_Profili_insmart_T20_quartieri">#REF!</definedName>
-    <definedName name="R_Share_perc">#REF!</definedName>
-    <definedName name="R_Speed_km_per_h">#REF!</definedName>
-    <definedName name="RetBE">[6]Macro1!#REF!</definedName>
-    <definedName name="RVP_and_beta">#REF!</definedName>
-    <definedName name="RVP_kPa">[7]RVP_kPa!$A$1:$B$13</definedName>
-    <definedName name="Selenium_Content_ppm_wt">#REF!</definedName>
-    <definedName name="Sulphur_Content_perc_wt">#REF!</definedName>
     <definedName name="table6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="Temperatures">#REF!</definedName>
-    <definedName name="tiket">#REF!</definedName>
-    <definedName name="TP.Electricity_and_RES">#REF!</definedName>
-    <definedName name="TP.Petroleum">#REF!</definedName>
-    <definedName name="TP.Solids_and_Gases">#REF!</definedName>
-    <definedName name="U_Share_perc">#REF!</definedName>
-    <definedName name="U_Speed_km_per_h">#REF!</definedName>
-    <definedName name="US.Electricity_and_RES">#REF!</definedName>
-    <definedName name="US.Petroleum">#REF!</definedName>
-    <definedName name="US.Solids_and_Gases">#REF!</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="yeare">#REF!</definedName>
-    <definedName name="yearf">#REF!</definedName>
-    <definedName name="yearg">#REF!</definedName>
-    <definedName name="Zinc_Content_ppm_wt">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1358,574 +1265,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Start"/>
-      <sheetName val="Cover"/>
-      <sheetName val="Menu"/>
-      <sheetName val="Table1"/>
-      <sheetName val="Table2"/>
-      <sheetName val="Table3"/>
-      <sheetName val="Table4"/>
-      <sheetName val="Table5"/>
-      <sheetName val="Table6a"/>
-      <sheetName val="Table6b"/>
-      <sheetName val="Table6c"/>
-      <sheetName val="Table6d"/>
-      <sheetName val="Table7a"/>
-      <sheetName val="Table7b"/>
-      <sheetName val="Table8"/>
-      <sheetName val="TableEU-1"/>
-      <sheetName val="TableEU-2"/>
-      <sheetName val="GELE"/>
-      <sheetName val="GHEAT"/>
-      <sheetName val="NELE"/>
-      <sheetName val="NHEAT"/>
-      <sheetName val="ELET34"/>
-      <sheetName val="HEAT34"/>
-      <sheetName val="TAB5ELE"/>
-      <sheetName val="TAB5CHP"/>
-      <sheetName val="TAB5TOT"/>
-      <sheetName val="TAB5HEAT"/>
-      <sheetName val="TAB5CHPH"/>
-      <sheetName val="TAB5TOTH"/>
-      <sheetName val="TAB6ANTONS"/>
-      <sheetName val="TAB6CCTONS"/>
-      <sheetName val="TAB6OBCTONS"/>
-      <sheetName val="TAB6SCTONS"/>
-      <sheetName val="TAB6LIGTONS"/>
-      <sheetName val="TAB6PEATONS"/>
-      <sheetName val="TAB6PFUELTONS"/>
-      <sheetName val="TAB6COKEOCTONS"/>
-      <sheetName val="TAB6GASCOKETONS"/>
-      <sheetName val="TAB6COALTARTONS"/>
-      <sheetName val="TAB6BKBTONS"/>
-      <sheetName val="TAB6GWGASTJ"/>
-      <sheetName val="TAB6COGTJ"/>
-      <sheetName val="TAB6BFGTJ"/>
-      <sheetName val="TAB6OSGASTJ"/>
-      <sheetName val="TAB6CRUDOILTONS"/>
-      <sheetName val="TAB6NGLTONS"/>
-      <sheetName val="TAB6REFGASTONS"/>
-      <sheetName val="TAB6LPGTONS"/>
-      <sheetName val="TAB6NAPHTHATONS"/>
-      <sheetName val="TAB6KERJETONS"/>
-      <sheetName val="TAB6OTHKEROTONS"/>
-      <sheetName val="TAB6GASDIESTONS"/>
-      <sheetName val="TAB6HFUELTONS"/>
-      <sheetName val="TAB6BITUTONS"/>
-      <sheetName val="TAB6PETCOKETONS"/>
-      <sheetName val="TAB6OTHOILTONS"/>
-      <sheetName val="TAB6NGASTJ"/>
-      <sheetName val="TAB6INDWTJ"/>
-      <sheetName val="TAB6MSWRTJ"/>
-      <sheetName val="TAB6MSWNRTJ"/>
-      <sheetName val="TAB6WOODTJ"/>
-      <sheetName val="TAB6LANDGASTJ"/>
-      <sheetName val="TAB6SEWAGETJ"/>
-      <sheetName val="TAB6OTHBIOTJ"/>
-      <sheetName val="TAB6LIQBIOTONS"/>
-      <sheetName val="TAB6TOTAL"/>
-      <sheetName val="TAB7MAIN"/>
-      <sheetName val="TAB7AUTO"/>
-      <sheetName val="TAB8IMPE"/>
-      <sheetName val="TAB8IMPHC"/>
-      <sheetName val="TAB8EXPE"/>
-      <sheetName val="TAB8EXPHC"/>
-      <sheetName val="Remarks"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="105">
-          <cell r="D105">
-            <v>2010</v>
-          </cell>
-        </row>
-        <row r="111">
-          <cell r="G111">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="117">
-          <cell r="G117">
-            <v>2010</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2">
-        <row r="42">
-          <cell r="AE42" t="str">
-            <v>Menu</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-      <sheetData sheetId="59"/>
-      <sheetData sheetId="60"/>
-      <sheetData sheetId="61"/>
-      <sheetData sheetId="62"/>
-      <sheetData sheetId="63"/>
-      <sheetData sheetId="64"/>
-      <sheetData sheetId="65"/>
-      <sheetData sheetId="66"/>
-      <sheetData sheetId="67"/>
-      <sheetData sheetId="68"/>
-      <sheetData sheetId="69"/>
-      <sheetData sheetId="70"/>
-      <sheetData sheetId="71"/>
-      <sheetData sheetId="72"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1">
-        <row r="4">
-          <cell r="C4" t="str">
-            <v>European Community</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover"/>
-      <sheetName val="Intro"/>
-      <sheetName val="EB2012"/>
-      <sheetName val="COM_Balance"/>
-      <sheetName val="COM_Commodities"/>
-      <sheetName val="COM_Processes"/>
-      <sheetName val="COM_FuelTechs"/>
-      <sheetName val="COM_EmiCoeffs"/>
-      <sheetName val="COM_CH"/>
-      <sheetName val="COM_CW"/>
-      <sheetName val="COM_CC"/>
-      <sheetName val="COM_CO"/>
-      <sheetName val="COM_PV"/>
-      <sheetName val="Commercial SEAI"/>
-      <sheetName val="Public SEAI"/>
-      <sheetName val="CSO data"/>
-      <sheetName val="Public BOC"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="7_Buildings managed by municipa"/>
-      <sheetName val="Tertiary"/>
-      <sheetName val="7_Buildings managed by muni (2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="IEA Data"/>
-      <sheetName val="E&amp;D Drivers"/>
-      <sheetName val="AGR_Fuels"/>
-      <sheetName val="AGR"/>
-      <sheetName val="RES_Fuels"/>
-      <sheetName val="RH1"/>
-      <sheetName val="RH2"/>
-      <sheetName val="RH3"/>
-      <sheetName val="RH4"/>
-      <sheetName val="RC1"/>
-      <sheetName val="RC2"/>
-      <sheetName val="RC3"/>
-      <sheetName val="RC4"/>
-      <sheetName val="RHW"/>
-      <sheetName val="RRF"/>
-      <sheetName val="RCW"/>
-      <sheetName val="RCD"/>
-      <sheetName val="RK1"/>
-      <sheetName val="RK2"/>
-      <sheetName val="RK3"/>
-      <sheetName val="RK4"/>
-      <sheetName val="RDW"/>
-      <sheetName val="RME"/>
-      <sheetName val="RL1"/>
-      <sheetName val="RL2"/>
-      <sheetName val="RL3"/>
-      <sheetName val="RL4"/>
-      <sheetName val="COM_Fuels"/>
-      <sheetName val="CH1"/>
-      <sheetName val="CH2"/>
-      <sheetName val="CH3"/>
-      <sheetName val="CH4"/>
-      <sheetName val="CC1"/>
-      <sheetName val="CC2"/>
-      <sheetName val="CC3"/>
-      <sheetName val="CC4"/>
-      <sheetName val="CHW"/>
-      <sheetName val="CAA"/>
-      <sheetName val="CLA"/>
-      <sheetName val="ElastPar"/>
-      <sheetName val="Conversion Factors"/>
-      <sheetName val="Intro"/>
-      <sheetName val="TechRep"/>
-      <sheetName val="Other_HYDRO"/>
-      <sheetName val="Other_NUCL"/>
-      <sheetName val="Other_THERM"/>
-      <sheetName val="Other_CHP"/>
-      <sheetName val="Other_RENEW"/>
-      <sheetName val="Other_HEAT"/>
-      <sheetName val="ELC_FUELS"/>
-      <sheetName val="ELC"/>
-      <sheetName val="HEAT"/>
-      <sheetName val="CHP"/>
-      <sheetName val="ELC_EMI"/>
-      <sheetName val="Constant Table"/>
-      <sheetName val="ANS_ITEMS_DEL"/>
-      <sheetName val="ANS_ITEMS"/>
-      <sheetName val="ANS_TIDDATA"/>
-      <sheetName val="ANS_TSDATA"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>^FI_ST: TCH, PRC</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Macro1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Population"/>
-      <sheetName val="Mileage_km"/>
-      <sheetName val="Mean_Fleet_Mileage_km"/>
-      <sheetName val="Fuel_Injection_perc"/>
-      <sheetName val="Evap_Control_perc"/>
-      <sheetName val="U_Speed_km_per_h"/>
-      <sheetName val="R_Speed_km_per_h"/>
-      <sheetName val="H_Speed_km_per_h"/>
-      <sheetName val="U_Share_perc"/>
-      <sheetName val="R_Share_perc"/>
-      <sheetName val="H_Share_perc"/>
-      <sheetName val="Evap_U_Share_perc"/>
-      <sheetName val="Evap_R_Share_perc"/>
-      <sheetName val="Evap_H_Share_perc"/>
-      <sheetName val="Min_Temperature_oC"/>
-      <sheetName val="Max_Temperature_oC"/>
-      <sheetName val="Temperatures"/>
-      <sheetName val="RVP_kPa"/>
-      <sheetName val="Beta"/>
-      <sheetName val="Fuel_Specifications"/>
-      <sheetName val="Improved_Fuel_Specs"/>
-      <sheetName val="Annual_Fuel_Consumption"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>Month_</v>
-          </cell>
-          <cell r="B1" t="str">
-            <v>2005</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>January</v>
-          </cell>
-          <cell r="B2">
-            <v>88.7</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>February</v>
-          </cell>
-          <cell r="B3">
-            <v>87.9</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>March</v>
-          </cell>
-          <cell r="B4">
-            <v>85.7</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>April</v>
-          </cell>
-          <cell r="B5">
-            <v>72.900000000000006</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>May</v>
-          </cell>
-          <cell r="B6">
-            <v>62.8</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>June</v>
-          </cell>
-          <cell r="B7">
-            <v>59.6</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>July</v>
-          </cell>
-          <cell r="B8">
-            <v>59.8</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>August</v>
-          </cell>
-          <cell r="B9">
-            <v>57</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>September</v>
-          </cell>
-          <cell r="B10">
-            <v>57.9</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>October</v>
-          </cell>
-          <cell r="B11">
-            <v>68.8</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>November</v>
-          </cell>
-          <cell r="B12">
-            <v>81.099999999999994</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>December</v>
-          </cell>
-          <cell r="B13">
-            <v>86.9</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4672,6 +4011,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F4935B8855D2CD4A84AB51A7B8A3B83B" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6046aa80c6137ea7cd300941e6de6139">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="795b6ce3-4d29-4fa5-96ed-ea1b36830f13" xmlns:ns3="424ab569-3a9e-4e02-994b-fd1ed8ea43ac" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8866ff8f472ea66287faba2f38092fc5" ns2:_="" ns3:_="">
     <xsd:import namespace="795b6ce3-4d29-4fa5-96ed-ea1b36830f13"/>
@@ -4850,22 +4204,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5D25AEF-5EEE-4730-89DA-F522B2580678}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C84C340F-40A4-4836-8E7A-67ECA799FFAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{087D185F-92EF-42F7-BB5C-65DF32C58C0D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4882,21 +4238,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C84C340F-40A4-4836-8E7A-67ECA799FFAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5D25AEF-5EEE-4730-89DA-F522B2580678}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>